<commit_message>
Export Excel | Consolidate Report Changes
</commit_message>
<xml_diff>
--- a/deliveryreview/Delivery_Review-01Dec_v0.1.xlsx
+++ b/deliveryreview/Delivery_Review-01Dec_v0.1.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Current Deployment" r:id="rId3" sheetId="1"/>
+    <sheet name="Bench Report" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3697" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3984" uniqueCount="307">
   <si>
     <t>Sr.No</t>
   </si>
@@ -495,6 +496,444 @@
   </si>
   <si>
     <t>17/11/2021</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Normalised Bench</t>
+  </si>
+  <si>
+    <t>Software Engg</t>
+  </si>
+  <si>
+    <t>5.32</t>
+  </si>
+  <si>
+    <t>1.65</t>
+  </si>
+  <si>
+    <t>4.00</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>3.23</t>
+  </si>
+  <si>
+    <t>1.03</t>
+  </si>
+  <si>
+    <t>3.09</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>10.18</t>
+  </si>
+  <si>
+    <t>3.05</t>
+  </si>
+  <si>
+    <t>13.43</t>
+  </si>
+  <si>
+    <t>4.03</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>Sen.Software Engg</t>
+  </si>
+  <si>
+    <t>4.86</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>1.27</t>
+  </si>
+  <si>
+    <t>6.41</t>
+  </si>
+  <si>
+    <t>2.50</t>
+  </si>
+  <si>
+    <t>7.83</t>
+  </si>
+  <si>
+    <t>9.00</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>1.72</t>
+  </si>
+  <si>
+    <t>0.18</t>
+  </si>
+  <si>
+    <t>0.16</t>
+  </si>
+  <si>
+    <t>2.45</t>
+  </si>
+  <si>
+    <t>2.11</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>1.34</t>
+  </si>
+  <si>
+    <t>2.58</t>
+  </si>
+  <si>
+    <t>9.68</t>
+  </si>
+  <si>
+    <t>8.23</t>
+  </si>
+  <si>
+    <t>11.22</t>
+  </si>
+  <si>
+    <t>9.53</t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>10.20</t>
+  </si>
+  <si>
+    <t>Sen.Technical Specialist</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>1.57</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>1.42</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>1.36</t>
+  </si>
+  <si>
+    <t>3.86</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
+    <t>5.28</t>
+  </si>
+  <si>
+    <t>2.82</t>
+  </si>
+  <si>
+    <t>4.96</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>3.60</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>0.09</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>8.68</t>
+  </si>
+  <si>
+    <t>14.59</t>
+  </si>
+  <si>
+    <t>15.12</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>16.80</t>
+  </si>
+  <si>
+    <t>Sen.Technical Architect</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>0.32</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>2.14</t>
+  </si>
+  <si>
+    <t>1.61</t>
+  </si>
+  <si>
+    <t>6.72</t>
+  </si>
+  <si>
+    <t>Princ.Technical Architect</t>
+  </si>
+  <si>
+    <t>2.98</t>
+  </si>
+  <si>
+    <t>2.41</t>
+  </si>
+  <si>
+    <t>2.34</t>
+  </si>
+  <si>
+    <t>2.28</t>
+  </si>
+  <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>3.24</t>
+  </si>
+  <si>
+    <t>4.54</t>
+  </si>
+  <si>
+    <t>4.48</t>
+  </si>
+  <si>
+    <t>Asso.Princ.Technical Architect</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>1.86</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>4.38</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>17.64</t>
+  </si>
+  <si>
+    <t>15.51</t>
+  </si>
+  <si>
+    <t>11.10</t>
+  </si>
+  <si>
+    <t>10.01</t>
+  </si>
+  <si>
+    <t>9.21</t>
+  </si>
+  <si>
+    <t>8.59</t>
+  </si>
+  <si>
+    <t>6.58</t>
+  </si>
+  <si>
+    <t>11.45</t>
+  </si>
+  <si>
+    <t>8.14</t>
+  </si>
+  <si>
+    <t>8.05</t>
+  </si>
+  <si>
+    <t>8.09</t>
+  </si>
+  <si>
+    <t>11.00</t>
+  </si>
+  <si>
+    <t>13.63</t>
+  </si>
+  <si>
+    <t>43.73</t>
+  </si>
+  <si>
+    <t>44.47</t>
+  </si>
+  <si>
+    <t>51.09</t>
+  </si>
+  <si>
+    <t>49.58</t>
+  </si>
+  <si>
+    <t>57.00</t>
+  </si>
+  <si>
+    <t>55.97</t>
+  </si>
+  <si>
+    <t>Simple Average</t>
+  </si>
+  <si>
+    <t>43%</t>
+  </si>
+  <si>
+    <t>38%</t>
+  </si>
+  <si>
+    <t>24%</t>
+  </si>
+  <si>
+    <t>21%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>18%</t>
+  </si>
+  <si>
+    <t>14%</t>
+  </si>
+  <si>
+    <t>22%</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>23%</t>
+  </si>
+  <si>
+    <t>74%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>87%</t>
+  </si>
+  <si>
+    <t>84%</t>
+  </si>
+  <si>
+    <t>97%</t>
+  </si>
+  <si>
+    <t>95%</t>
   </si>
 </sst>
 </file>
@@ -502,7 +941,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -534,6 +973,21 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
     </font>
   </fonts>
   <fills count="8">
@@ -604,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
@@ -619,6 +1073,15 @@
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyFill="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -12110,4 +12573,931 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:Y12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="3" max="3" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="17.34375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="27.82421875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="6">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s" s="7">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s" s="7">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s" s="7">
+        <v>164</v>
+      </c>
+      <c r="H1" t="s" s="7">
+        <v>165</v>
+      </c>
+      <c r="J1" t="s" s="7">
+        <v>166</v>
+      </c>
+      <c r="L1" t="s" s="7">
+        <v>167</v>
+      </c>
+      <c r="N1" t="s" s="7">
+        <v>168</v>
+      </c>
+      <c r="P1" t="s" s="7">
+        <v>169</v>
+      </c>
+      <c r="R1" t="s" s="7">
+        <v>170</v>
+      </c>
+      <c r="T1" t="s" s="7">
+        <v>171</v>
+      </c>
+      <c r="V1" t="s" s="7">
+        <v>172</v>
+      </c>
+      <c r="X1" t="s" s="7">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="C2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="D2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="E2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="G2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="H2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="I2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="J2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="K2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="L2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="M2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="N2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="O2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="P2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="Q2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="R2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="S2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="T2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="U2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="V2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="W2" t="s" s="7">
+        <v>175</v>
+      </c>
+      <c r="X2" t="s" s="7">
+        <v>174</v>
+      </c>
+      <c r="Y2" t="s" s="7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="8">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s" s="6">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s" s="6">
+        <v>179</v>
+      </c>
+      <c r="E3" t="s" s="6">
+        <v>180</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>181</v>
+      </c>
+      <c r="G3" t="s" s="6">
+        <v>182</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>183</v>
+      </c>
+      <c r="I3" t="s" s="6">
+        <v>184</v>
+      </c>
+      <c r="J3" t="s" s="6">
+        <v>179</v>
+      </c>
+      <c r="K3" t="s" s="6">
+        <v>185</v>
+      </c>
+      <c r="L3" t="s" s="6">
+        <v>186</v>
+      </c>
+      <c r="M3" t="s" s="6">
+        <v>187</v>
+      </c>
+      <c r="N3" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="O3" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="P3" t="s" s="6">
+        <v>189</v>
+      </c>
+      <c r="Q3" t="s" s="6">
+        <v>190</v>
+      </c>
+      <c r="R3" t="s" s="6">
+        <v>191</v>
+      </c>
+      <c r="S3" t="s" s="6">
+        <v>192</v>
+      </c>
+      <c r="T3" t="s" s="6">
+        <v>193</v>
+      </c>
+      <c r="U3" t="s" s="6">
+        <v>194</v>
+      </c>
+      <c r="V3" t="s" s="6">
+        <v>193</v>
+      </c>
+      <c r="W3" t="s" s="6">
+        <v>194</v>
+      </c>
+      <c r="X3" t="s" s="6">
+        <v>193</v>
+      </c>
+      <c r="Y3" t="s" s="6">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="8">
+        <v>195</v>
+      </c>
+      <c r="B4" t="s" s="6">
+        <v>196</v>
+      </c>
+      <c r="C4" t="s" s="6">
+        <v>197</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>198</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>199</v>
+      </c>
+      <c r="F4" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="G4" t="s" s="6">
+        <v>201</v>
+      </c>
+      <c r="H4" t="s" s="6">
+        <v>183</v>
+      </c>
+      <c r="I4" t="s" s="6">
+        <v>202</v>
+      </c>
+      <c r="J4" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>185</v>
+      </c>
+      <c r="L4" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="M4" t="s" s="6">
+        <v>185</v>
+      </c>
+      <c r="N4" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="O4" t="s" s="6">
+        <v>185</v>
+      </c>
+      <c r="P4" t="s" s="6">
+        <v>203</v>
+      </c>
+      <c r="Q4" t="s" s="6">
+        <v>204</v>
+      </c>
+      <c r="R4" t="s" s="6">
+        <v>205</v>
+      </c>
+      <c r="S4" t="s" s="6">
+        <v>190</v>
+      </c>
+      <c r="T4" t="s" s="6">
+        <v>206</v>
+      </c>
+      <c r="U4" t="s" s="6">
+        <v>207</v>
+      </c>
+      <c r="V4" t="s" s="6">
+        <v>206</v>
+      </c>
+      <c r="W4" t="s" s="6">
+        <v>207</v>
+      </c>
+      <c r="X4" t="s" s="6">
+        <v>206</v>
+      </c>
+      <c r="Y4" t="s" s="6">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="8">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>208</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>209</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="F5" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="G5" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="H5" t="s" s="6">
+        <v>210</v>
+      </c>
+      <c r="I5" t="s" s="6">
+        <v>211</v>
+      </c>
+      <c r="J5" t="s" s="6">
+        <v>212</v>
+      </c>
+      <c r="K5" t="s" s="6">
+        <v>213</v>
+      </c>
+      <c r="L5" t="s" s="6">
+        <v>214</v>
+      </c>
+      <c r="M5" t="s" s="6">
+        <v>215</v>
+      </c>
+      <c r="N5" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="O5" t="s" s="6">
+        <v>216</v>
+      </c>
+      <c r="P5" t="s" s="6">
+        <v>217</v>
+      </c>
+      <c r="Q5" t="s" s="6">
+        <v>218</v>
+      </c>
+      <c r="R5" t="s" s="6">
+        <v>219</v>
+      </c>
+      <c r="S5" t="s" s="6">
+        <v>220</v>
+      </c>
+      <c r="T5" t="s" s="6">
+        <v>221</v>
+      </c>
+      <c r="U5" t="s" s="6">
+        <v>222</v>
+      </c>
+      <c r="V5" t="s" s="6">
+        <v>221</v>
+      </c>
+      <c r="W5" t="s" s="6">
+        <v>222</v>
+      </c>
+      <c r="X5" t="s" s="6">
+        <v>221</v>
+      </c>
+      <c r="Y5" t="s" s="6">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="8">
+        <v>223</v>
+      </c>
+      <c r="B6" t="s" s="6">
+        <v>224</v>
+      </c>
+      <c r="C6" t="s" s="6">
+        <v>225</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="E6" t="s" s="6">
+        <v>227</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="G6" t="s" s="6">
+        <v>227</v>
+      </c>
+      <c r="H6" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="I6" t="s" s="6">
+        <v>228</v>
+      </c>
+      <c r="J6" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="K6" t="s" s="6">
+        <v>229</v>
+      </c>
+      <c r="L6" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="M6" t="s" s="6">
+        <v>230</v>
+      </c>
+      <c r="N6" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="O6" t="s" s="6">
+        <v>215</v>
+      </c>
+      <c r="P6" t="s" s="6">
+        <v>231</v>
+      </c>
+      <c r="Q6" t="s" s="6">
+        <v>232</v>
+      </c>
+      <c r="R6" t="s" s="6">
+        <v>179</v>
+      </c>
+      <c r="S6" t="s" s="6">
+        <v>233</v>
+      </c>
+      <c r="T6" t="s" s="6">
+        <v>179</v>
+      </c>
+      <c r="U6" t="s" s="6">
+        <v>233</v>
+      </c>
+      <c r="V6" t="s" s="6">
+        <v>179</v>
+      </c>
+      <c r="W6" t="s" s="6">
+        <v>233</v>
+      </c>
+      <c r="X6" t="s" s="6">
+        <v>179</v>
+      </c>
+      <c r="Y6" t="s" s="6">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="8">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s" s="6">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s" s="6">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="E7" t="s" s="6">
+        <v>237</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>238</v>
+      </c>
+      <c r="G7" t="s" s="6">
+        <v>239</v>
+      </c>
+      <c r="H7" t="s" s="6">
+        <v>240</v>
+      </c>
+      <c r="I7" t="s" s="6">
+        <v>211</v>
+      </c>
+      <c r="J7" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="K7" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="L7" t="s" s="6">
+        <v>210</v>
+      </c>
+      <c r="M7" t="s" s="6">
+        <v>241</v>
+      </c>
+      <c r="N7" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="O7" t="s" s="6">
+        <v>242</v>
+      </c>
+      <c r="P7" t="s" s="6">
+        <v>243</v>
+      </c>
+      <c r="Q7" t="s" s="6">
+        <v>244</v>
+      </c>
+      <c r="R7" t="s" s="6">
+        <v>206</v>
+      </c>
+      <c r="S7" t="s" s="6">
+        <v>245</v>
+      </c>
+      <c r="T7" t="s" s="6">
+        <v>246</v>
+      </c>
+      <c r="U7" t="s" s="6">
+        <v>247</v>
+      </c>
+      <c r="V7" t="s" s="6">
+        <v>246</v>
+      </c>
+      <c r="W7" t="s" s="6">
+        <v>247</v>
+      </c>
+      <c r="X7" t="s" s="6">
+        <v>246</v>
+      </c>
+      <c r="Y7" t="s" s="6">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="8">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s" s="6">
+        <v>249</v>
+      </c>
+      <c r="C8" t="s" s="6">
+        <v>250</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="G8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="H8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="I8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="J8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="K8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="L8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="M8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="N8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="O8" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="P8" t="s" s="6">
+        <v>251</v>
+      </c>
+      <c r="Q8" t="s" s="6">
+        <v>252</v>
+      </c>
+      <c r="R8" t="s" s="6">
+        <v>253</v>
+      </c>
+      <c r="S8" t="s" s="6">
+        <v>237</v>
+      </c>
+      <c r="T8" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="U8" t="s" s="6">
+        <v>254</v>
+      </c>
+      <c r="V8" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="W8" t="s" s="6">
+        <v>254</v>
+      </c>
+      <c r="X8" t="s" s="6">
+        <v>200</v>
+      </c>
+      <c r="Y8" t="s" s="6">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="8">
+        <v>255</v>
+      </c>
+      <c r="B9" t="s" s="6">
+        <v>202</v>
+      </c>
+      <c r="C9" t="s" s="6">
+        <v>256</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="E9" t="s" s="6">
+        <v>257</v>
+      </c>
+      <c r="F9" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="G9" t="s" s="6">
+        <v>257</v>
+      </c>
+      <c r="H9" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="I9" t="s" s="6">
+        <v>258</v>
+      </c>
+      <c r="J9" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="K9" t="s" s="6">
+        <v>259</v>
+      </c>
+      <c r="L9" t="s" s="6">
+        <v>260</v>
+      </c>
+      <c r="M9" t="s" s="6">
+        <v>261</v>
+      </c>
+      <c r="N9" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="O9" t="s" s="6">
+        <v>262</v>
+      </c>
+      <c r="P9" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="Q9" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="R9" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="S9" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="T9" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="U9" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="V9" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="W9" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="X9" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="Y9" t="s" s="6">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="8">
+        <v>264</v>
+      </c>
+      <c r="B10" t="s" s="6">
+        <v>249</v>
+      </c>
+      <c r="C10" t="s" s="6">
+        <v>250</v>
+      </c>
+      <c r="D10" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="E10" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s" s="6">
+        <v>265</v>
+      </c>
+      <c r="G10" t="s" s="6">
+        <v>266</v>
+      </c>
+      <c r="H10" t="s" s="6">
+        <v>249</v>
+      </c>
+      <c r="I10" t="s" s="6">
+        <v>250</v>
+      </c>
+      <c r="J10" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="K10" t="s" s="6">
+        <v>188</v>
+      </c>
+      <c r="L10" t="s" s="6">
+        <v>210</v>
+      </c>
+      <c r="M10" t="s" s="6">
+        <v>267</v>
+      </c>
+      <c r="N10" t="s" s="6">
+        <v>226</v>
+      </c>
+      <c r="O10" t="s" s="6">
+        <v>268</v>
+      </c>
+      <c r="P10" t="s" s="6">
+        <v>208</v>
+      </c>
+      <c r="Q10" t="s" s="6">
+        <v>269</v>
+      </c>
+      <c r="R10" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="S10" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="T10" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="U10" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="V10" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="W10" t="s" s="6">
+        <v>263</v>
+      </c>
+      <c r="X10" t="s" s="6">
+        <v>236</v>
+      </c>
+      <c r="Y10" t="s" s="6">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="6">
+        <v>270</v>
+      </c>
+      <c r="B11" t="s" s="6">
+        <v>271</v>
+      </c>
+      <c r="C11" t="s" s="6">
+        <v>272</v>
+      </c>
+      <c r="D11" t="s" s="6">
+        <v>273</v>
+      </c>
+      <c r="E11" t="s" s="6">
+        <v>274</v>
+      </c>
+      <c r="F11" t="s" s="6">
+        <v>217</v>
+      </c>
+      <c r="G11" t="s" s="6">
+        <v>275</v>
+      </c>
+      <c r="H11" t="s" s="6">
+        <v>276</v>
+      </c>
+      <c r="I11" t="s" s="6">
+        <v>277</v>
+      </c>
+      <c r="J11" t="s" s="6">
+        <v>278</v>
+      </c>
+      <c r="K11" t="s" s="6">
+        <v>279</v>
+      </c>
+      <c r="L11" t="s" s="6">
+        <v>280</v>
+      </c>
+      <c r="M11" t="s" s="6">
+        <v>281</v>
+      </c>
+      <c r="N11" t="s" s="6">
+        <v>282</v>
+      </c>
+      <c r="O11" t="s" s="6">
+        <v>283</v>
+      </c>
+      <c r="P11" t="s" s="6">
+        <v>284</v>
+      </c>
+      <c r="Q11" t="s" s="6">
+        <v>285</v>
+      </c>
+      <c r="R11" t="s" s="6">
+        <v>286</v>
+      </c>
+      <c r="S11" t="s" s="6">
+        <v>287</v>
+      </c>
+      <c r="T11" t="s" s="6">
+        <v>288</v>
+      </c>
+      <c r="U11" t="s" s="6">
+        <v>289</v>
+      </c>
+      <c r="V11" t="s" s="6">
+        <v>288</v>
+      </c>
+      <c r="W11" t="s" s="6">
+        <v>289</v>
+      </c>
+      <c r="X11" t="s" s="6">
+        <v>288</v>
+      </c>
+      <c r="Y11" t="s" s="6">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="6">
+        <v>290</v>
+      </c>
+      <c r="B12" t="s" s="6">
+        <v>291</v>
+      </c>
+      <c r="C12" t="s" s="8">
+        <v>292</v>
+      </c>
+      <c r="D12" t="s" s="6">
+        <v>293</v>
+      </c>
+      <c r="E12" t="s" s="8">
+        <v>294</v>
+      </c>
+      <c r="F12" t="s" s="6">
+        <v>294</v>
+      </c>
+      <c r="G12" t="s" s="8">
+        <v>295</v>
+      </c>
+      <c r="H12" t="s" s="6">
+        <v>296</v>
+      </c>
+      <c r="I12" t="s" s="8">
+        <v>297</v>
+      </c>
+      <c r="J12" t="s" s="6">
+        <v>298</v>
+      </c>
+      <c r="K12" t="s" s="8">
+        <v>299</v>
+      </c>
+      <c r="L12" t="s" s="6">
+        <v>299</v>
+      </c>
+      <c r="M12" t="s" s="8">
+        <v>299</v>
+      </c>
+      <c r="N12" t="s" s="6">
+        <v>296</v>
+      </c>
+      <c r="O12" t="s" s="8">
+        <v>300</v>
+      </c>
+      <c r="P12" t="s" s="6">
+        <v>301</v>
+      </c>
+      <c r="Q12" t="s" s="8">
+        <v>302</v>
+      </c>
+      <c r="R12" t="s" s="6">
+        <v>303</v>
+      </c>
+      <c r="S12" t="s" s="8">
+        <v>304</v>
+      </c>
+      <c r="T12" t="s" s="6">
+        <v>305</v>
+      </c>
+      <c r="U12" t="s" s="8">
+        <v>306</v>
+      </c>
+      <c r="V12" t="s" s="6">
+        <v>305</v>
+      </c>
+      <c r="W12" t="s" s="8">
+        <v>306</v>
+      </c>
+      <c r="X12" t="s" s="6">
+        <v>305</v>
+      </c>
+      <c r="Y12" t="s" s="8">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>